<commit_message>
data uderstanding selesai, menambahkan descrinbe data belum clean di tabel 4.1 dan 4.2
</commit_message>
<xml_diff>
--- a/data/Tabel 4.1.xlsx
+++ b/data/Tabel 4.1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Hp\Desktop\rainfall-prediction\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9A8FA1DB-2B8A-48DF-B3A6-11F6438A1988}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E5BB238-A3D8-475A-936B-0B5408C324AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1515" yWindow="1515" windowWidth="15375" windowHeight="7995" xr2:uid="{E662CDAE-9B0A-4EC8-B854-E1DB9C96DC01}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{E662CDAE-9B0A-4EC8-B854-E1DB9C96DC01}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="73">
   <si>
     <t>Air Tmp (C) M 60 Min</t>
   </si>
@@ -162,13 +162,106 @@
   </si>
   <si>
     <t>3.0</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Mag WD 60 Min (deg) M</t>
+  </si>
+  <si>
+    <t>True WD 60 Min (deg) M</t>
+  </si>
+  <si>
+    <t>klasifikasi</t>
+  </si>
+  <si>
+    <t>82.0</t>
+  </si>
+  <si>
+    <t>29.7</t>
+  </si>
+  <si>
+    <t>84.0</t>
+  </si>
+  <si>
+    <t>rain</t>
+  </si>
+  <si>
+    <t>61.0</t>
+  </si>
+  <si>
+    <t>29.5</t>
+  </si>
+  <si>
+    <t>63.0</t>
+  </si>
+  <si>
+    <t>23.5</t>
+  </si>
+  <si>
+    <t>5.0</t>
+  </si>
+  <si>
+    <t>340.0</t>
+  </si>
+  <si>
+    <t>21.9</t>
+  </si>
+  <si>
+    <t>342.0</t>
+  </si>
+  <si>
+    <t>297.0</t>
+  </si>
+  <si>
+    <t>19.9</t>
+  </si>
+  <si>
+    <t>299.0</t>
+  </si>
+  <si>
+    <t>269.0</t>
+  </si>
+  <si>
+    <t>NaN</t>
+  </si>
+  <si>
+    <t>271.0</t>
+  </si>
+  <si>
+    <t>no rain</t>
+  </si>
+  <si>
+    <t>301.0</t>
+  </si>
+  <si>
+    <t>303.0</t>
+  </si>
+  <si>
+    <t>312.0</t>
+  </si>
+  <si>
+    <t>314.0</t>
+  </si>
+  <si>
+    <t>334.0</t>
+  </si>
+  <si>
+    <t>336.0</t>
+  </si>
+  <si>
+    <t>331.0</t>
+  </si>
+  <si>
+    <t>333.0</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -186,6 +279,20 @@
       <sz val="11"/>
       <name val="Segoe UI"/>
       <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -223,7 +330,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
@@ -233,6 +340,13 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -548,165 +662,181 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E72569C-876B-455D-920F-7F7896E4FB59}">
-  <dimension ref="A2:G13"/>
+  <dimension ref="A2:J27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:G13"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="L18" sqref="L18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.28515625" customWidth="1"/>
-    <col min="2" max="2" width="12" customWidth="1"/>
-    <col min="3" max="3" width="11" customWidth="1"/>
-    <col min="4" max="4" width="12" customWidth="1"/>
-    <col min="5" max="5" width="10.7109375" customWidth="1"/>
-    <col min="6" max="6" width="10.42578125" customWidth="1"/>
-    <col min="7" max="7" width="14.85546875" customWidth="1"/>
+    <col min="2" max="2" width="22.28515625" customWidth="1"/>
+    <col min="3" max="3" width="12" customWidth="1"/>
+    <col min="4" max="4" width="11" customWidth="1"/>
+    <col min="5" max="5" width="12" customWidth="1"/>
+    <col min="6" max="6" width="10.7109375" customWidth="1"/>
+    <col min="7" max="7" width="10.42578125" customWidth="1"/>
+    <col min="8" max="8" width="14.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:7" ht="66" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+    <row r="2" spans="1:10" ht="49.5" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="C2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="G2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="H2" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="33" x14ac:dyDescent="0.25">
-      <c r="A3" s="2">
+    <row r="3" spans="1:10" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A3" s="4">
+        <v>1</v>
+      </c>
+      <c r="B3" s="2">
         <v>44896</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="C3" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="D3" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="E3" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="F3" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="F3" s="3" t="s">
+      <c r="G3" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="G3" s="3" t="s">
+      <c r="H3" s="3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="33" x14ac:dyDescent="0.25">
-      <c r="A4" s="2">
+    <row r="4" spans="1:10" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A4" s="4">
+        <v>2</v>
+      </c>
+      <c r="B4" s="2">
         <v>44896.041666666664</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="C4" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="D4" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="E4" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="F4" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="G4" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="G4" s="3" t="s">
+      <c r="H4" s="3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="33" x14ac:dyDescent="0.25">
-      <c r="A5" s="2">
+    <row r="5" spans="1:10" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A5" s="4">
+        <v>3</v>
+      </c>
+      <c r="B5" s="2">
         <v>44896.083333333336</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="C5" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="D5" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="E5" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="E5" s="3" t="s">
+      <c r="F5" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="F5" s="3" t="s">
+      <c r="G5" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="G5" s="3" t="s">
+      <c r="H5" s="3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="33" x14ac:dyDescent="0.25">
-      <c r="A6" s="2">
+    <row r="6" spans="1:10" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A6" s="4">
+        <v>4</v>
+      </c>
+      <c r="B6" s="2">
         <v>44896.125</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="C6" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="D6" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="E6" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="E6" s="3" t="s">
+      <c r="F6" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="F6" s="3" t="s">
+      <c r="G6" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="G6" s="3" t="s">
+      <c r="H6" s="3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="33" x14ac:dyDescent="0.25">
-      <c r="A7" s="2">
+    <row r="7" spans="1:10" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A7" s="4">
+        <v>5</v>
+      </c>
+      <c r="B7" s="2">
         <v>44896.166666666664</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="C7" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="D7" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D7" s="3" t="s">
+      <c r="E7" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="E7" s="3" t="s">
+      <c r="F7" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="F7" s="3" t="s">
+      <c r="G7" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="G7" s="3" t="s">
+      <c r="H7" s="3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
-        <v>26</v>
-      </c>
+    <row r="8" spans="1:10" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A8" s="4"/>
       <c r="B8" s="3" t="s">
         <v>26</v>
       </c>
@@ -725,120 +855,522 @@
       <c r="G8" s="3" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" ht="33" x14ac:dyDescent="0.25">
-      <c r="A9" s="2">
+      <c r="H8" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A9" s="4">
+        <v>2036</v>
+      </c>
+      <c r="B9" s="2">
         <v>44980.791666666664</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="C9" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="D9" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D9" s="3" t="s">
+      <c r="E9" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="E9" s="3" t="s">
+      <c r="F9" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="F9" s="3" t="s">
+      <c r="G9" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="G9" s="3" t="s">
+      <c r="H9" s="3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="33" x14ac:dyDescent="0.25">
-      <c r="A10" s="2">
+    <row r="10" spans="1:10" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A10" s="4">
+        <v>2037</v>
+      </c>
+      <c r="B10" s="2">
         <v>44980.833333333336</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="C10" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="D10" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D10" s="3" t="s">
+      <c r="E10" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="E10" s="3" t="s">
+      <c r="F10" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="F10" s="3" t="s">
+      <c r="G10" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="G10" s="3" t="s">
+      <c r="H10" s="3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="33" x14ac:dyDescent="0.25">
-      <c r="A11" s="2">
+    <row r="11" spans="1:10" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A11" s="4">
+        <v>2038</v>
+      </c>
+      <c r="B11" s="2">
         <v>44980.875</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="C11" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="C11" s="3" t="s">
+      <c r="D11" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D11" s="3" t="s">
+      <c r="E11" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="E11" s="3" t="s">
+      <c r="F11" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="F11" s="3" t="s">
+      <c r="G11" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="G11" s="3" t="s">
+      <c r="H11" s="3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="33" x14ac:dyDescent="0.25">
-      <c r="A12" s="2">
+    <row r="12" spans="1:10" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A12" s="4">
+        <v>2039</v>
+      </c>
+      <c r="B12" s="2">
         <v>44980.916666666664</v>
       </c>
-      <c r="B12" s="3" t="s">
+      <c r="C12" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="C12" s="3" t="s">
+      <c r="D12" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D12" s="3" t="s">
+      <c r="E12" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="E12" s="3" t="s">
+      <c r="F12" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="F12" s="3" t="s">
+      <c r="G12" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="G12" s="3" t="s">
+      <c r="H12" s="3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="33" x14ac:dyDescent="0.25">
-      <c r="A13" s="2">
+    <row r="13" spans="1:10" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A13" s="4">
+        <v>2040</v>
+      </c>
+      <c r="B13" s="2">
         <v>44980.958333333336</v>
       </c>
-      <c r="B13" s="3" t="s">
+      <c r="C13" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="C13" s="3" t="s">
+      <c r="D13" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D13" s="3" t="s">
+      <c r="E13" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="E13" s="3" t="s">
+      <c r="F13" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="F13" s="3" t="s">
+      <c r="G13" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="G13" s="3" t="s">
+      <c r="H13" s="3" t="s">
         <v>12</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" ht="49.5" x14ac:dyDescent="0.25">
+      <c r="A16" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="I16" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="J16" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A17" s="3">
+        <v>0</v>
+      </c>
+      <c r="B17" s="2">
+        <v>44896</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="F17" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G17" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="H17" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="I17" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="J17" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A18" s="3">
+        <v>1</v>
+      </c>
+      <c r="B18" s="2">
+        <v>44896.041666666664</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="F18" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="G18" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="H18" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="I18" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="J18" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A19" s="3">
+        <v>2</v>
+      </c>
+      <c r="B19" s="2">
+        <v>44896.083333333336</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="F19" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G19" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="H19" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="I19" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="J19" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A20" s="3">
+        <v>3</v>
+      </c>
+      <c r="B20" s="2">
+        <v>44896.125</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="F20" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G20" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="H20" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="I20" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="J20" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A21" s="3">
+        <v>4</v>
+      </c>
+      <c r="B21" s="2">
+        <v>44896.166666666664</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="E21" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="F21" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="G21" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="H21" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="I21" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="J21" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A22" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="E22" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="F22" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="G22" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="H22" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="I22" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="J22" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A23" s="3">
+        <v>2035</v>
+      </c>
+      <c r="B23" s="2">
+        <v>44980.791666666664</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="E23" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="F23" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="G23" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="H23" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="I23" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="J23" s="3" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A24" s="3">
+        <v>2036</v>
+      </c>
+      <c r="B24" s="2">
+        <v>44980.833333333336</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="E24" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="F24" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="G24" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="H24" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="I24" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="J24" s="3" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A25" s="3">
+        <v>2037</v>
+      </c>
+      <c r="B25" s="2">
+        <v>44980.875</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="E25" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="F25" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="G25" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="H25" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="I25" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="J25" s="3" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A26" s="3">
+        <v>2038</v>
+      </c>
+      <c r="B26" s="2">
+        <v>44980.916666666664</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="E26" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="F26" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="G26" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="H26" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="I26" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="J26" s="3" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A27" s="3">
+        <v>2039</v>
+      </c>
+      <c r="B27" s="2">
+        <v>44980.958333333336</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="E27" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="F27" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="G27" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="H27" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="I27" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="J27" s="3" t="s">
+        <v>64</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add file skripsi, tambah fitur importance, dan dataset full
</commit_message>
<xml_diff>
--- a/data/Tabel 4.1.xlsx
+++ b/data/Tabel 4.1.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Hp\Desktop\rainfall-prediction\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E5BB238-A3D8-475A-936B-0B5408C324AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D73C413-5535-4E7A-AA61-2247F974289E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{E662CDAE-9B0A-4EC8-B854-E1DB9C96DC01}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="68">
   <si>
     <t>Air Tmp (C) M 60 Min</t>
   </si>
@@ -179,9 +179,6 @@
     <t>82.0</t>
   </si>
   <si>
-    <t>29.7</t>
-  </si>
-  <si>
     <t>84.0</t>
   </si>
   <si>
@@ -191,31 +188,19 @@
     <t>61.0</t>
   </si>
   <si>
-    <t>29.5</t>
-  </si>
-  <si>
     <t>63.0</t>
   </si>
   <si>
-    <t>23.5</t>
-  </si>
-  <si>
     <t>5.0</t>
   </si>
   <si>
     <t>340.0</t>
   </si>
   <si>
-    <t>21.9</t>
-  </si>
-  <si>
     <t>342.0</t>
   </si>
   <si>
     <t>297.0</t>
-  </si>
-  <si>
-    <t>19.9</t>
   </si>
   <si>
     <t>299.0</t>
@@ -664,8 +649,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E72569C-876B-455D-920F-7F7896E4FB59}">
   <dimension ref="A2:J27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="L18" sqref="L18"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17:I21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1035,7 +1020,7 @@
         <v>46</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>47</v>
+        <v>8</v>
       </c>
       <c r="F17" s="3" t="s">
         <v>9</v>
@@ -1044,13 +1029,13 @@
         <v>10</v>
       </c>
       <c r="H17" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="I17" s="3" t="s">
         <v>11</v>
       </c>
       <c r="J17" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="18" spans="1:10" ht="16.5" x14ac:dyDescent="0.25">
@@ -1064,10 +1049,10 @@
         <v>13</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>51</v>
+        <v>8</v>
       </c>
       <c r="F18" s="3" t="s">
         <v>14</v>
@@ -1076,13 +1061,13 @@
         <v>15</v>
       </c>
       <c r="H18" s="3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="I18" s="3" t="s">
         <v>11</v>
       </c>
       <c r="J18" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="19" spans="1:10" ht="16.5" x14ac:dyDescent="0.25">
@@ -1099,7 +1084,7 @@
         <v>41</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>53</v>
+        <v>8</v>
       </c>
       <c r="F19" s="3" t="s">
         <v>17</v>
@@ -1108,13 +1093,13 @@
         <v>18</v>
       </c>
       <c r="H19" s="3" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="I19" s="3" t="s">
         <v>11</v>
       </c>
       <c r="J19" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="20" spans="1:10" ht="16.5" x14ac:dyDescent="0.25">
@@ -1128,10 +1113,10 @@
         <v>19</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>56</v>
+        <v>8</v>
       </c>
       <c r="F20" s="3" t="s">
         <v>20</v>
@@ -1140,13 +1125,13 @@
         <v>21</v>
       </c>
       <c r="H20" s="3" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="I20" s="3" t="s">
         <v>11</v>
       </c>
       <c r="J20" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="21" spans="1:10" ht="16.5" x14ac:dyDescent="0.25">
@@ -1160,10 +1145,10 @@
         <v>22</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="F21" s="3" t="s">
         <v>23</v>
@@ -1172,13 +1157,13 @@
         <v>24</v>
       </c>
       <c r="H21" s="3" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="I21" s="3" t="s">
         <v>25</v>
       </c>
       <c r="J21" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="22" spans="1:10" ht="16.5" x14ac:dyDescent="0.25">
@@ -1224,10 +1209,10 @@
         <v>27</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="F23" s="3" t="s">
         <v>28</v>
@@ -1236,13 +1221,13 @@
         <v>29</v>
       </c>
       <c r="H23" s="3" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="I23" s="3" t="s">
         <v>11</v>
       </c>
       <c r="J23" s="3" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
     </row>
     <row r="24" spans="1:10" ht="16.5" x14ac:dyDescent="0.25">
@@ -1256,10 +1241,10 @@
         <v>30</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="F24" s="3" t="s">
         <v>31</v>
@@ -1268,13 +1253,13 @@
         <v>32</v>
       </c>
       <c r="H24" s="3" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="I24" s="3" t="s">
         <v>11</v>
       </c>
       <c r="J24" s="3" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
     </row>
     <row r="25" spans="1:10" ht="16.5" x14ac:dyDescent="0.25">
@@ -1288,10 +1273,10 @@
         <v>33</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="F25" s="3" t="s">
         <v>34</v>
@@ -1300,13 +1285,13 @@
         <v>15</v>
       </c>
       <c r="H25" s="3" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="I25" s="3" t="s">
         <v>11</v>
       </c>
       <c r="J25" s="3" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
     </row>
     <row r="26" spans="1:10" ht="16.5" x14ac:dyDescent="0.25">
@@ -1320,10 +1305,10 @@
         <v>35</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="F26" s="3" t="s">
         <v>36</v>
@@ -1332,13 +1317,13 @@
         <v>37</v>
       </c>
       <c r="H26" s="3" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="I26" s="3" t="s">
         <v>25</v>
       </c>
       <c r="J26" s="3" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
     </row>
     <row r="27" spans="1:10" ht="16.5" x14ac:dyDescent="0.25">
@@ -1352,10 +1337,10 @@
         <v>38</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="F27" s="3" t="s">
         <v>39</v>
@@ -1364,13 +1349,13 @@
         <v>40</v>
       </c>
       <c r="H27" s="3" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="I27" s="3" t="s">
         <v>41</v>
       </c>
       <c r="J27" s="3" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
     </row>
   </sheetData>

</xml_diff>